<commit_message>
updating maps, adding local council data
</commit_message>
<xml_diff>
--- a/data-raw/party_colour.xlsx
+++ b/data-raw/party_colour.xlsx
@@ -1,33 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanodell/Documents/GitHub/parlitools/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eodell\Documents\GitHub\parlitools\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16245" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t>Alliance</t>
   </si>
@@ -255,13 +252,22 @@
   </si>
   <si>
     <t>UKIP</t>
+  </si>
+  <si>
+    <t>noc</t>
+  </si>
+  <si>
+    <t>No Overall Control</t>
+  </si>
+  <si>
+    <t>#231f20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,16 +275,314 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -286,22 +590,219 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="41" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="44">
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="20" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="24" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="28" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="32" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="36" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="40" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="21" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="25" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="29" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="33" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="37" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="15" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="43"/>
+    <cellStyle name="Normal 3" xfId="41"/>
+    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -570,535 +1071,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>41</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>43</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>44</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>46</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>47</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>50</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>51</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>52</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>53</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>